<commit_message>
226090 Add unpublish action for items tab
</commit_message>
<xml_diff>
--- a/tests/product_files/PRD-1234-1234-1234-file-update.xlsx
+++ b/tests/product_files/PRD-1234-1234-1234-file-update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavellonkin/Documents/git/swo-marketplace-cli/tests/product_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CBF1DF-A0A5-AC43-A481-CA0DD00FCBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D61AD5E-541B-2748-A7BD-CABC082A7321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="131">
   <si>
     <t>General Information</t>
   </si>
@@ -482,6 +482,12 @@
   </si>
   <si>
     <t>ITM-1213-3316-0004</t>
+  </si>
+  <si>
+    <t>ITM-1213-3316-0005</t>
+  </si>
+  <si>
+    <t>unpublish</t>
   </si>
 </sst>
 </file>
@@ -2017,10 +2023,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2321,10 +2327,66 @@
         <v>45292</v>
       </c>
     </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" t="s">
+        <v>93</v>
+      </c>
+      <c r="N6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" t="s">
+        <v>98</v>
+      </c>
+      <c r="P6" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>45292</v>
+      </c>
+      <c r="R6" s="5">
+        <v>45292</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C5" xr:uid="{00000000-0002-0000-0700-000000000000}">
-      <formula1>"-,update,review,publish"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{7B8F7546-DF62-5A4E-A30B-2255272A291A}">
+      <formula1>"-,update,review,publish,unpublish"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
226091 Add create action for item, when product definition is updated
</commit_message>
<xml_diff>
--- a/tests/product_files/PRD-1234-1234-1234-file-update.xlsx
+++ b/tests/product_files/PRD-1234-1234-1234-file-update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavellonkin/Documents/git/swo-marketplace-cli/tests/product_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D61AD5E-541B-2748-A7BD-CABC082A7321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4567284-25BD-3844-B9B1-7CEA2387725C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="136">
   <si>
     <t>General Information</t>
   </si>
@@ -488,6 +488,21 @@
   </si>
   <si>
     <t>unpublish</t>
+  </si>
+  <si>
+    <t>ITM-1213-3316-0006</t>
+  </si>
+  <si>
+    <t>65AB123BASD2</t>
+  </si>
+  <si>
+    <t>NAV123456</t>
+  </si>
+  <si>
+    <t>Description 6</t>
+  </si>
+  <si>
+    <t>create</t>
   </si>
 </sst>
 </file>
@@ -2023,10 +2038,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2383,10 +2398,66 @@
         <v>45292</v>
       </c>
     </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" t="s">
+        <v>92</v>
+      </c>
+      <c r="M7" t="s">
+        <v>93</v>
+      </c>
+      <c r="N7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" t="s">
+        <v>98</v>
+      </c>
+      <c r="P7" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>45292</v>
+      </c>
+      <c r="R7" s="5">
+        <v>45292</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{7B8F7546-DF62-5A4E-A30B-2255272A291A}">
-      <formula1>"-,update,review,publish,unpublish"</formula1>
+      <formula1>"-,create,update,review,publish,unpublish"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
226154 User vendor item ID to work with actions in Items tab
</commit_message>
<xml_diff>
--- a/tests/product_files/PRD-1234-1234-1234-file-update.xlsx
+++ b/tests/product_files/PRD-1234-1234-1234-file-update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavellonkin/Documents/git/swo-marketplace-cli/tests/product_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4567284-25BD-3844-B9B1-7CEA2387725C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC80678-701B-FE42-8CEE-D09CA2B6A7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -922,7 +922,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2041,7 +2041,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>